<commit_message>
Work in active (#2144)
* should be able to filter work as active/inactive/all

* create_work not working
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/minister_designation/002_Minister_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/minister_designation/002_Minister_Designation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91EBDCC-E964-4592-815E-19A900ED0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAD8864-4847-4CC3-ABF1-0263C5421051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -1255,7 +1255,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1937,11 +1937,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M183"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A58" sqref="A58:E136"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -3661,7 +3661,7 @@
         <v>23</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="I43" s="11" t="b">
         <v>0</v>
@@ -5164,11 +5164,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20:E30"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -5885,10 +5885,10 @@
   <dimension ref="A1:G197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -9451,15 +9451,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
@@ -9468,6 +9459,15 @@
     <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9700,20 +9700,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E491705-4376-42A3-B308-4EDB544680E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A969FC-83AB-41B8-867D-F5874D3E25B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
     <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E491705-4376-42A3-B308-4EDB544680E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
minister designation template fix
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/minister_designation/002_Minister_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/minister_designation/002_Minister_Designation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAD8864-4847-4CC3-ABF1-0263C5421051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A17603-F51D-4B4F-8F13-278E5CF34B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Action_Temp" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Actions!$D$1:$D$197</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Actions!$D$1:$D$199</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Events!$A$1:$M$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$E$15</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="202">
   <si>
     <t>No</t>
   </si>
@@ -656,12 +656,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -842,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -859,14 +866,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -875,7 +882,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -887,16 +894,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -905,45 +912,46 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,7 +1263,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1331,7 +1339,7 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="37" t="s">
         <v>145</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1937,11 +1945,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -5882,13 +5890,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G197"/>
+  <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15:G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -6363,20 +6371,20 @@
         <v>20</v>
       </c>
       <c r="B20" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
+        <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="G20" s="2">
         <v>20</v>
@@ -6394,13 +6402,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G21" s="2">
         <v>21</v>
@@ -6418,13 +6426,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>184</v>
+        <v>83</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G22" s="2">
         <v>22</v>
@@ -6435,20 +6443,20 @@
         <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="4" t="str">
         <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Minister to make the Minister's Designation Decision</v>
+        <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>141</v>
+        <v>87</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>184</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G23" s="2">
         <v>23</v>
@@ -6459,20 +6467,20 @@
         <v>24</v>
       </c>
       <c r="B24" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="4" t="str">
         <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO is delegated to make the Minister's Designation Decision</v>
+        <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G24" s="2">
         <v>24</v>
@@ -6483,20 +6491,20 @@
         <v>25</v>
       </c>
       <c r="B25" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" s="4" t="str">
         <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
+        <v>Minister to make the Minister's Designation Decision</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G25" s="2">
         <v>25</v>
@@ -6507,20 +6515,20 @@
         <v>26</v>
       </c>
       <c r="B26" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>82</v>
+        <v>CEAO is delegated to make the Minister's Designation Decision</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="G26" s="2">
         <v>26</v>
@@ -6537,14 +6545,14 @@
         <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>87</v>
+      <c r="D27" t="s">
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G27" s="2">
         <v>27</v>
@@ -6562,13 +6570,13 @@
         <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G28" s="2">
         <v>28</v>
@@ -6579,20 +6587,20 @@
         <v>29</v>
       </c>
       <c r="B29" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" s="4" t="str">
         <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
-      </c>
-      <c r="D29" t="s">
-        <v>83</v>
+        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G29" s="2">
         <v>29</v>
@@ -6603,20 +6611,20 @@
         <v>30</v>
       </c>
       <c r="B30" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" s="4" t="str">
         <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G30" s="2">
         <v>30</v>
@@ -6633,14 +6641,14 @@
         <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>87</v>
+      <c r="D31" t="s">
+        <v>83</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G31" s="2">
         <v>31</v>
@@ -6658,13 +6666,13 @@
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G32" s="2">
         <v>32</v>
@@ -6675,20 +6683,20 @@
         <v>33</v>
       </c>
       <c r="B33" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" s="4" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>EAO's Viewpoint is POSITIVE</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>140</v>
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="G33" s="2">
         <v>33</v>
@@ -6699,20 +6707,20 @@
         <v>34</v>
       </c>
       <c r="B34" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C34" s="4" t="str">
         <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>EAO's Viewpoint is NEGATIVE</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>140</v>
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>89</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="G34" s="2">
         <v>34</v>
@@ -6723,20 +6731,20 @@
         <v>35</v>
       </c>
       <c r="B35" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" s="4" t="str">
         <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
-      </c>
-      <c r="D35" t="s">
-        <v>83</v>
+        <v>EAO's Viewpoint is POSITIVE</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G35" s="2">
         <v>35</v>
@@ -6747,20 +6755,20 @@
         <v>36</v>
       </c>
       <c r="B36" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="4" t="str">
         <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>82</v>
+        <v>EAO's Viewpoint is NEGATIVE</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G36" s="2">
         <v>36</v>
@@ -6777,14 +6785,14 @@
         <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D37" s="24" t="s">
-        <v>87</v>
+      <c r="D37" t="s">
+        <v>83</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G37" s="2">
         <v>37</v>
@@ -6802,13 +6810,13 @@
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G38" s="2">
         <v>38</v>
@@ -6819,20 +6827,20 @@
         <v>39</v>
       </c>
       <c r="B39" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="4" t="str">
         <f>IF((B39=""),"",VLOOKUP(B39,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D39" t="s">
-        <v>83</v>
+      <c r="D39" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G39" s="2">
         <v>39</v>
@@ -6843,20 +6851,20 @@
         <v>40</v>
       </c>
       <c r="B40" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="4" t="str">
         <f>IF((B40=""),"",VLOOKUP(B40,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G40" s="2">
         <v>40</v>
@@ -6873,14 +6881,14 @@
         <f>IF((B41=""),"",VLOOKUP(B41,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D41" s="24" t="s">
-        <v>87</v>
+      <c r="D41" t="s">
+        <v>83</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G41" s="2">
         <v>41</v>
@@ -6898,13 +6906,13 @@
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G42" s="2">
         <v>42</v>
@@ -6915,20 +6923,20 @@
         <v>43</v>
       </c>
       <c r="B43" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="4" t="str">
         <f>IF((B43=""),"",VLOOKUP(B43,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Designates Project as Reviewable</v>
-      </c>
-      <c r="D43" s="1" t="s">
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D43" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E43" s="32" t="s">
-        <v>184</v>
+      <c r="E43" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G43" s="2">
         <v>43</v>
@@ -6939,20 +6947,20 @@
         <v>44</v>
       </c>
       <c r="B44" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" s="4" t="str">
         <f>IF((B44=""),"",VLOOKUP(B44,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Designates Project as Reviewable</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>185</v>
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G44" s="2">
         <v>44</v>
@@ -6963,11 +6971,11 @@
         <v>45</v>
       </c>
       <c r="B45" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="4" t="str">
         <f>IF((B45=""),"",VLOOKUP(B45,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Declines to Designate Project as Reviewable</v>
+        <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>87</v>
@@ -6987,20 +6995,20 @@
         <v>46</v>
       </c>
       <c r="B46" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="4" t="str">
         <f>IF((B46=""),"",VLOOKUP(B46,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Declines to Designate Project as Reviewable</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>143</v>
+        <v>Decision Maker Designates Project as Reviewable</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G46" s="2">
         <v>46</v>
@@ -7010,8 +7018,22 @@
       <c r="A47" s="2">
         <v>47</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="3">
+        <v>18</v>
+      </c>
+      <c r="C47" s="4" t="str">
+        <f>IF((B47=""),"",VLOOKUP(B47,Outcomes!$A$2:$D$30,4,FALSE))</f>
+        <v>Decision Maker Declines to Designate Project as Reviewable</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="G47" s="2">
         <v>47</v>
       </c>
@@ -7020,742 +7042,560 @@
       <c r="A48" s="2">
         <v>48</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
+      <c r="B48" s="3">
+        <v>18</v>
+      </c>
+      <c r="C48" s="4" t="str">
+        <f>IF((B48=""),"",VLOOKUP(B48,Outcomes!$A$2:$D$30,4,FALSE))</f>
+        <v>Decision Maker Declines to Designate Project as Reviewable</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="G48" s="2">
         <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="2">
-        <v>49</v>
-      </c>
+      <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
-      <c r="E49" s="32"/>
-      <c r="G49" s="2">
-        <v>49</v>
-      </c>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="2">
-        <v>50</v>
-      </c>
+      <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="G50" s="2">
-        <v>50</v>
-      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="2">
-        <v>51</v>
-      </c>
+      <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
-      <c r="G51" s="2">
-        <v>51</v>
-      </c>
+      <c r="E51" s="32"/>
+      <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="2">
-        <v>52</v>
-      </c>
+      <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
-      <c r="G52" s="2">
-        <v>52</v>
-      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="2">
-        <v>53</v>
-      </c>
+      <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
-      <c r="G53" s="2">
-        <v>53</v>
-      </c>
+      <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="2">
-        <v>54</v>
-      </c>
+      <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
-      <c r="G54" s="2">
-        <v>54</v>
-      </c>
+      <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="2">
-        <v>55</v>
-      </c>
+      <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
-      <c r="G55" s="2">
-        <v>55</v>
-      </c>
+      <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="2">
-        <v>56</v>
-      </c>
+      <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
-      <c r="G56" s="2">
-        <v>56</v>
-      </c>
+      <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="2">
-        <v>57</v>
-      </c>
+      <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
-      <c r="G57" s="2">
-        <v>57</v>
-      </c>
+      <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="2">
-        <v>58</v>
-      </c>
+      <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="4"/>
-      <c r="G58" s="2">
-        <v>58</v>
-      </c>
+      <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="2">
-        <v>59</v>
-      </c>
+      <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
-      <c r="G59" s="2">
-        <v>59</v>
-      </c>
+      <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="2">
-        <v>60</v>
-      </c>
+      <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
-      <c r="G60" s="2">
-        <v>60</v>
-      </c>
+      <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="2">
-        <v>61</v>
-      </c>
+      <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4"/>
-      <c r="G61" s="2">
-        <v>61</v>
-      </c>
+      <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="2">
-        <v>62</v>
-      </c>
+      <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
-      <c r="G62" s="2">
-        <v>62</v>
-      </c>
+      <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="2">
-        <v>63</v>
-      </c>
+      <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="4"/>
-      <c r="G63" s="2">
-        <v>63</v>
-      </c>
+      <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="2">
-        <v>64</v>
-      </c>
+      <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
-      <c r="G64" s="2">
-        <v>64</v>
-      </c>
+      <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="2">
-        <v>65</v>
-      </c>
+      <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
-      <c r="G65" s="2">
-        <v>65</v>
-      </c>
+      <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="2">
-        <v>66</v>
-      </c>
+      <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="4"/>
-      <c r="G66" s="2">
-        <v>66</v>
-      </c>
+      <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="2">
-        <v>67</v>
-      </c>
+      <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
-      <c r="G67" s="2">
-        <v>67</v>
-      </c>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="2">
-        <v>68</v>
-      </c>
+      <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="4"/>
-      <c r="G68" s="2">
-        <v>68</v>
-      </c>
+      <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="2">
-        <v>69</v>
-      </c>
+      <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="4"/>
-      <c r="G69" s="2">
-        <v>69</v>
-      </c>
+      <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="2">
-        <v>70</v>
-      </c>
+      <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="4"/>
-      <c r="G70" s="2">
-        <v>70</v>
-      </c>
+      <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="2">
-        <v>71</v>
-      </c>
+      <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="4"/>
-      <c r="G71" s="2">
-        <v>71</v>
-      </c>
+      <c r="G71" s="2"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="2">
-        <v>72</v>
-      </c>
+      <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
-      <c r="G72" s="2">
-        <v>72</v>
-      </c>
+      <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="2">
-        <v>73</v>
-      </c>
+      <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="4"/>
-      <c r="G73" s="2">
-        <v>73</v>
-      </c>
+      <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="2">
-        <v>74</v>
-      </c>
+      <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="4"/>
-      <c r="G74" s="2">
-        <v>74</v>
-      </c>
+      <c r="G74" s="2"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="2">
-        <v>75</v>
-      </c>
+      <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
-      <c r="G75" s="2">
-        <v>75</v>
-      </c>
+      <c r="G75" s="2"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="2">
-        <v>76</v>
-      </c>
+      <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
-      <c r="G76" s="2">
-        <v>76</v>
-      </c>
+      <c r="G76" s="2"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="2">
-        <v>77</v>
-      </c>
+      <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
-      <c r="G77" s="2">
-        <v>77</v>
-      </c>
+      <c r="G77" s="2"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="2">
-        <v>78</v>
-      </c>
+      <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
-      <c r="G78" s="2">
-        <v>78</v>
-      </c>
+      <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="2">
-        <v>79</v>
-      </c>
+      <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
-      <c r="G79" s="2">
-        <v>79</v>
-      </c>
+      <c r="G79" s="2"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="2">
-        <v>80</v>
-      </c>
+      <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
-      <c r="G80" s="2">
-        <v>80</v>
-      </c>
+      <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="2">
-        <v>81</v>
-      </c>
+      <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="4"/>
-      <c r="G81" s="2">
-        <v>81</v>
-      </c>
+      <c r="G81" s="2"/>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="2">
-        <v>82</v>
-      </c>
+      <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
-      <c r="G82" s="2">
-        <v>82</v>
-      </c>
+      <c r="G82" s="2"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="2">
-        <v>83</v>
-      </c>
+      <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="4"/>
-      <c r="G83" s="2">
-        <v>83</v>
-      </c>
+      <c r="G83" s="2"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="2">
-        <v>84</v>
-      </c>
+      <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="4"/>
-      <c r="G84" s="2">
-        <v>84</v>
-      </c>
+      <c r="G84" s="2"/>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="2">
-        <v>85</v>
-      </c>
+      <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
-      <c r="G85" s="2">
-        <v>85</v>
-      </c>
+      <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="2">
-        <v>86</v>
-      </c>
+      <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="4"/>
-      <c r="G86" s="2">
-        <v>86</v>
-      </c>
+      <c r="G86" s="2"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="2">
-        <v>87</v>
-      </c>
+      <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="4"/>
-      <c r="G87" s="2">
-        <v>87</v>
-      </c>
+      <c r="G87" s="2"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="2">
-        <v>88</v>
-      </c>
+      <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="4"/>
-      <c r="G88" s="2">
-        <v>88</v>
-      </c>
+      <c r="G88" s="2"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="2">
-        <v>89</v>
-      </c>
+      <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
-      <c r="G89" s="2">
-        <v>89</v>
-      </c>
+      <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="2">
-        <v>90</v>
-      </c>
+      <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="4"/>
-      <c r="G90" s="2">
-        <v>90</v>
-      </c>
+      <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="2">
-        <v>91</v>
-      </c>
+      <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="4"/>
-      <c r="G91" s="2">
-        <v>91</v>
-      </c>
+      <c r="G91" s="2"/>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="2">
-        <v>92</v>
-      </c>
+      <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="4"/>
-      <c r="G92" s="2">
-        <v>92</v>
-      </c>
+      <c r="G92" s="2"/>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="2">
-        <v>93</v>
-      </c>
+      <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="4"/>
-      <c r="G93" s="2">
-        <v>93</v>
-      </c>
+      <c r="G93" s="2"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="2">
-        <v>94</v>
-      </c>
+      <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="4"/>
-      <c r="G94" s="2">
-        <v>94</v>
-      </c>
+      <c r="G94" s="2"/>
     </row>
     <row r="95" spans="1:7">
-      <c r="A95" s="2">
-        <v>95</v>
-      </c>
+      <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="4"/>
-      <c r="G95" s="2">
-        <v>95</v>
-      </c>
+      <c r="G95" s="2"/>
     </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="2">
-        <v>96</v>
-      </c>
+      <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="4"/>
-      <c r="G96" s="2">
-        <v>96</v>
-      </c>
+      <c r="G96" s="2"/>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="2">
-        <v>97</v>
-      </c>
+      <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="4"/>
-      <c r="G97" s="2">
-        <v>97</v>
-      </c>
+      <c r="G97" s="2"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="2">
-        <v>98</v>
-      </c>
+      <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="4"/>
-      <c r="G98" s="2">
-        <v>98</v>
-      </c>
+      <c r="G98" s="2"/>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="2">
-        <v>99</v>
-      </c>
+      <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="4"/>
-      <c r="G99" s="2">
-        <v>99</v>
-      </c>
+      <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="2">
-        <v>100</v>
-      </c>
+      <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="4"/>
-      <c r="D100"/>
-      <c r="G100" s="2">
-        <v>100</v>
-      </c>
+      <c r="G100" s="2"/>
     </row>
     <row r="101" spans="1:7">
-      <c r="D101" s="24"/>
+      <c r="A101" s="2"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="4"/>
+      <c r="G101" s="2"/>
     </row>
     <row r="102" spans="1:7">
-      <c r="D102" s="24"/>
+      <c r="A102" s="2"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="4"/>
+      <c r="D102"/>
+      <c r="G102" s="2"/>
     </row>
     <row r="103" spans="1:7">
       <c r="D103" s="24"/>
     </row>
-    <row r="106" spans="1:7">
-      <c r="D106" s="24"/>
+    <row r="104" spans="1:7">
+      <c r="D104" s="24"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="D105" s="24"/>
     </row>
     <row r="108" spans="1:7">
-      <c r="E108" s="25"/>
+      <c r="D108" s="24"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="D110"/>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="D111" s="24"/>
+      <c r="E110" s="25"/>
     </row>
     <row r="112" spans="1:7">
-      <c r="D112" s="24"/>
+      <c r="D112"/>
     </row>
     <row r="113" spans="4:4">
       <c r="D113" s="24"/>
     </row>
     <row r="114" spans="4:4">
-      <c r="D114"/>
+      <c r="D114" s="24"/>
     </row>
     <row r="115" spans="4:4">
       <c r="D115" s="24"/>
     </row>
     <row r="116" spans="4:4">
-      <c r="D116" s="24"/>
+      <c r="D116"/>
     </row>
     <row r="117" spans="4:4">
       <c r="D117" s="24"/>
     </row>
     <row r="118" spans="4:4">
-      <c r="D118" s="9"/>
-    </row>
-    <row r="121" spans="4:4">
-      <c r="D121"/>
-    </row>
-    <row r="122" spans="4:4">
-      <c r="D122" s="24"/>
+      <c r="D118" s="24"/>
+    </row>
+    <row r="119" spans="4:4">
+      <c r="D119" s="24"/>
+    </row>
+    <row r="120" spans="4:4">
+      <c r="D120" s="9"/>
     </row>
     <row r="123" spans="4:4">
-      <c r="D123" s="24"/>
+      <c r="D123"/>
     </row>
     <row r="124" spans="4:4">
       <c r="D124" s="24"/>
     </row>
     <row r="125" spans="4:4">
-      <c r="D125"/>
+      <c r="D125" s="24"/>
     </row>
     <row r="126" spans="4:4">
       <c r="D126" s="24"/>
     </row>
     <row r="127" spans="4:4">
-      <c r="D127" s="24"/>
+      <c r="D127"/>
     </row>
     <row r="128" spans="4:4">
       <c r="D128" s="24"/>
     </row>
     <row r="129" spans="4:5">
-      <c r="D129" s="25"/>
-      <c r="E129" s="25"/>
-    </row>
-    <row r="132" spans="4:5">
-      <c r="E132" s="25"/>
+      <c r="D129" s="24"/>
+    </row>
+    <row r="130" spans="4:5">
+      <c r="D130" s="24"/>
+    </row>
+    <row r="131" spans="4:5">
+      <c r="D131" s="25"/>
+      <c r="E131" s="25"/>
     </row>
     <row r="134" spans="4:5">
       <c r="E134" s="25"/>
     </row>
-    <row r="137" spans="4:5">
-      <c r="D137"/>
-    </row>
-    <row r="138" spans="4:5">
-      <c r="D138" s="24"/>
+    <row r="136" spans="4:5">
+      <c r="E136" s="25"/>
     </row>
     <row r="139" spans="4:5">
-      <c r="D139" s="24"/>
+      <c r="D139"/>
     </row>
     <row r="140" spans="4:5">
       <c r="D140" s="24"/>
     </row>
     <row r="141" spans="4:5">
-      <c r="D141"/>
+      <c r="D141" s="24"/>
     </row>
     <row r="142" spans="4:5">
       <c r="D142" s="24"/>
     </row>
     <row r="143" spans="4:5">
-      <c r="D143" s="24"/>
+      <c r="D143"/>
     </row>
     <row r="144" spans="4:5">
       <c r="D144" s="24"/>
     </row>
     <row r="145" spans="4:5">
-      <c r="D145" s="25"/>
-      <c r="E145" s="25"/>
+      <c r="D145" s="24"/>
     </row>
     <row r="146" spans="4:5">
-      <c r="D146"/>
+      <c r="D146" s="24"/>
     </row>
     <row r="147" spans="4:5">
-      <c r="D147" s="24"/>
+      <c r="D147" s="25"/>
+      <c r="E147" s="25"/>
     </row>
     <row r="148" spans="4:5">
-      <c r="D148" s="24"/>
+      <c r="D148"/>
     </row>
     <row r="149" spans="4:5">
       <c r="D149" s="24"/>
     </row>
+    <row r="150" spans="4:5">
+      <c r="D150" s="24"/>
+    </row>
     <row r="151" spans="4:5">
-      <c r="E151" s="25"/>
-    </row>
-    <row r="152" spans="4:5">
-      <c r="D152" s="9"/>
-      <c r="E152" s="25"/>
+      <c r="D151" s="24"/>
     </row>
     <row r="153" spans="4:5">
       <c r="E153" s="25"/>
     </row>
     <row r="154" spans="4:5">
-      <c r="D154" s="25"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="25"/>
     </row>
     <row r="155" spans="4:5">
-      <c r="D155"/>
+      <c r="E155" s="25"/>
     </row>
     <row r="156" spans="4:5">
-      <c r="D156" s="24"/>
+      <c r="D156" s="25"/>
     </row>
     <row r="157" spans="4:5">
-      <c r="D157" s="24"/>
+      <c r="D157"/>
     </row>
     <row r="158" spans="4:5">
       <c r="D158" s="24"/>
     </row>
     <row r="159" spans="4:5">
-      <c r="D159"/>
+      <c r="D159" s="24"/>
     </row>
     <row r="160" spans="4:5">
       <c r="D160" s="24"/>
     </row>
     <row r="161" spans="4:5">
-      <c r="D161" s="24"/>
+      <c r="D161"/>
     </row>
     <row r="162" spans="4:5">
       <c r="D162" s="24"/>
     </row>
-    <row r="165" spans="4:5">
-      <c r="E165" s="25"/>
+    <row r="163" spans="4:5">
+      <c r="D163" s="24"/>
+    </row>
+    <row r="164" spans="4:5">
+      <c r="D164" s="24"/>
     </row>
     <row r="167" spans="4:5">
       <c r="E167" s="25"/>
     </row>
-    <row r="168" spans="4:5">
-      <c r="E168" s="25"/>
-    </row>
     <row r="169" spans="4:5">
       <c r="E169" s="25"/>
     </row>
-    <row r="175" spans="4:5">
-      <c r="E175" s="25"/>
+    <row r="170" spans="4:5">
+      <c r="E170" s="25"/>
+    </row>
+    <row r="171" spans="4:5">
+      <c r="E171" s="25"/>
     </row>
     <row r="177" spans="4:5">
       <c r="E177" s="25"/>
     </row>
-    <row r="178" spans="4:5">
-      <c r="E178" s="25"/>
-    </row>
     <row r="179" spans="4:5">
       <c r="E179" s="25"/>
     </row>
-    <row r="185" spans="4:5">
-      <c r="E185" s="25"/>
-    </row>
-    <row r="186" spans="4:5">
-      <c r="E186" s="25"/>
+    <row r="180" spans="4:5">
+      <c r="E180" s="25"/>
+    </row>
+    <row r="181" spans="4:5">
+      <c r="E181" s="25"/>
     </row>
     <row r="187" spans="4:5">
-      <c r="D187"/>
+      <c r="E187" s="25"/>
     </row>
     <row r="188" spans="4:5">
-      <c r="D188" s="24"/>
+      <c r="E188" s="25"/>
     </row>
     <row r="189" spans="4:5">
-      <c r="D189" s="24"/>
+      <c r="D189"/>
     </row>
     <row r="190" spans="4:5">
       <c r="D190" s="24"/>
     </row>
+    <row r="191" spans="4:5">
+      <c r="D191" s="24"/>
+    </row>
     <row r="192" spans="4:5">
-      <c r="D192" s="25"/>
-    </row>
-    <row r="193" spans="4:4">
-      <c r="D193" s="24"/>
-    </row>
-    <row r="197" spans="4:4">
-      <c r="D197"/>
+      <c r="D192" s="24"/>
+    </row>
+    <row r="194" spans="4:4">
+      <c r="D194" s="25"/>
+    </row>
+    <row r="195" spans="4:4">
+      <c r="D195" s="24"/>
+    </row>
+    <row r="199" spans="4:4">
+      <c r="D199"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D197" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <autoFilter ref="D1:D199" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -7765,13 +7605,13 @@
           <x14:formula1>
             <xm:f>Lookups!$U$3:$U$16</xm:f>
           </x14:formula1>
-          <xm:sqref>D154:D212 D51:D149 D23:D42 D46 D2:D15</xm:sqref>
+          <xm:sqref>D156:D214 D53:D151 D24:D44 D48 D2:D15 D20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Outcomes!$A$2:$A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B100</xm:sqref>
+          <xm:sqref>B2:B102</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
minister designation template fix (#2148)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/minister_designation/002_Minister_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/minister_designation/002_Minister_Designation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAD8864-4847-4CC3-ABF1-0263C5421051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A17603-F51D-4B4F-8F13-278E5CF34B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Action_Temp" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Actions!$D$1:$D$197</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Actions!$D$1:$D$199</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Events!$A$1:$M$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$E$15</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="202">
   <si>
     <t>No</t>
   </si>
@@ -656,12 +656,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -842,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -859,14 +866,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -875,7 +882,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -887,16 +894,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -905,45 +912,46 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,7 +1263,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1331,7 +1339,7 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="37" t="s">
         <v>145</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1937,11 +1945,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -5882,13 +5890,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G197"/>
+  <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15:G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -6363,20 +6371,20 @@
         <v>20</v>
       </c>
       <c r="B20" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>IF((B20=""),"",VLOOKUP(B20,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
+        <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="G20" s="2">
         <v>20</v>
@@ -6394,13 +6402,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G21" s="2">
         <v>21</v>
@@ -6418,13 +6426,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>184</v>
+        <v>83</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G22" s="2">
         <v>22</v>
@@ -6435,20 +6443,20 @@
         <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="4" t="str">
         <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Minister to make the Minister's Designation Decision</v>
+        <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>141</v>
+        <v>87</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>184</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G23" s="2">
         <v>23</v>
@@ -6459,20 +6467,20 @@
         <v>24</v>
       </c>
       <c r="B24" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="4" t="str">
         <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO is delegated to make the Minister's Designation Decision</v>
+        <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G24" s="2">
         <v>24</v>
@@ -6483,20 +6491,20 @@
         <v>25</v>
       </c>
       <c r="B25" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" s="4" t="str">
         <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
+        <v>Minister to make the Minister's Designation Decision</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G25" s="2">
         <v>25</v>
@@ -6507,20 +6515,20 @@
         <v>26</v>
       </c>
       <c r="B26" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>82</v>
+        <v>CEAO is delegated to make the Minister's Designation Decision</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="G26" s="2">
         <v>26</v>
@@ -6537,14 +6545,14 @@
         <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>87</v>
+      <c r="D27" t="s">
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G27" s="2">
         <v>27</v>
@@ -6562,13 +6570,13 @@
         <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G28" s="2">
         <v>28</v>
@@ -6579,20 +6587,20 @@
         <v>29</v>
       </c>
       <c r="B29" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" s="4" t="str">
         <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
-      </c>
-      <c r="D29" t="s">
-        <v>83</v>
+        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G29" s="2">
         <v>29</v>
@@ -6603,20 +6611,20 @@
         <v>30</v>
       </c>
       <c r="B30" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" s="4" t="str">
         <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+        <v>Minister's Designation request is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G30" s="2">
         <v>30</v>
@@ -6633,14 +6641,14 @@
         <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>87</v>
+      <c r="D31" t="s">
+        <v>83</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G31" s="2">
         <v>31</v>
@@ -6658,13 +6666,13 @@
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G32" s="2">
         <v>32</v>
@@ -6675,20 +6683,20 @@
         <v>33</v>
       </c>
       <c r="B33" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" s="4" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>EAO's Viewpoint is POSITIVE</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>140</v>
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="G33" s="2">
         <v>33</v>
@@ -6699,20 +6707,20 @@
         <v>34</v>
       </c>
       <c r="B34" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C34" s="4" t="str">
         <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>EAO's Viewpoint is NEGATIVE</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>140</v>
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>89</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="G34" s="2">
         <v>34</v>
@@ -6723,20 +6731,20 @@
         <v>35</v>
       </c>
       <c r="B35" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" s="4" t="str">
         <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
-      </c>
-      <c r="D35" t="s">
-        <v>83</v>
+        <v>EAO's Viewpoint is POSITIVE</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G35" s="2">
         <v>35</v>
@@ -6747,20 +6755,20 @@
         <v>36</v>
       </c>
       <c r="B36" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="4" t="str">
         <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>82</v>
+        <v>EAO's Viewpoint is NEGATIVE</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G36" s="2">
         <v>36</v>
@@ -6777,14 +6785,14 @@
         <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D37" s="24" t="s">
-        <v>87</v>
+      <c r="D37" t="s">
+        <v>83</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G37" s="2">
         <v>37</v>
@@ -6802,13 +6810,13 @@
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G38" s="2">
         <v>38</v>
@@ -6819,20 +6827,20 @@
         <v>39</v>
       </c>
       <c r="B39" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="4" t="str">
         <f>IF((B39=""),"",VLOOKUP(B39,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D39" t="s">
-        <v>83</v>
+      <c r="D39" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G39" s="2">
         <v>39</v>
@@ -6843,20 +6851,20 @@
         <v>40</v>
       </c>
       <c r="B40" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="4" t="str">
         <f>IF((B40=""),"",VLOOKUP(B40,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G40" s="2">
         <v>40</v>
@@ -6873,14 +6881,14 @@
         <f>IF((B41=""),"",VLOOKUP(B41,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
-      <c r="D41" s="24" t="s">
-        <v>87</v>
+      <c r="D41" t="s">
+        <v>83</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G41" s="2">
         <v>41</v>
@@ -6898,13 +6906,13 @@
         <v>Proponent Withdraws Project from the Minister's Designation Process</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G42" s="2">
         <v>42</v>
@@ -6915,20 +6923,20 @@
         <v>43</v>
       </c>
       <c r="B43" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="4" t="str">
         <f>IF((B43=""),"",VLOOKUP(B43,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Designates Project as Reviewable</v>
-      </c>
-      <c r="D43" s="1" t="s">
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D43" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E43" s="32" t="s">
-        <v>184</v>
+      <c r="E43" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G43" s="2">
         <v>43</v>
@@ -6939,20 +6947,20 @@
         <v>44</v>
       </c>
       <c r="B44" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" s="4" t="str">
         <f>IF((B44=""),"",VLOOKUP(B44,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Designates Project as Reviewable</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>185</v>
+        <v>Proponent Withdraws Project from the Minister's Designation Process</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G44" s="2">
         <v>44</v>
@@ -6963,11 +6971,11 @@
         <v>45</v>
       </c>
       <c r="B45" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="4" t="str">
         <f>IF((B45=""),"",VLOOKUP(B45,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Declines to Designate Project as Reviewable</v>
+        <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>87</v>
@@ -6987,20 +6995,20 @@
         <v>46</v>
       </c>
       <c r="B46" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="4" t="str">
         <f>IF((B46=""),"",VLOOKUP(B46,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Decision Maker Declines to Designate Project as Reviewable</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>143</v>
+        <v>Decision Maker Designates Project as Reviewable</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G46" s="2">
         <v>46</v>
@@ -7010,8 +7018,22 @@
       <c r="A47" s="2">
         <v>47</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="3">
+        <v>18</v>
+      </c>
+      <c r="C47" s="4" t="str">
+        <f>IF((B47=""),"",VLOOKUP(B47,Outcomes!$A$2:$D$30,4,FALSE))</f>
+        <v>Decision Maker Declines to Designate Project as Reviewable</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="G47" s="2">
         <v>47</v>
       </c>
@@ -7020,742 +7042,560 @@
       <c r="A48" s="2">
         <v>48</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
+      <c r="B48" s="3">
+        <v>18</v>
+      </c>
+      <c r="C48" s="4" t="str">
+        <f>IF((B48=""),"",VLOOKUP(B48,Outcomes!$A$2:$D$30,4,FALSE))</f>
+        <v>Decision Maker Declines to Designate Project as Reviewable</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="G48" s="2">
         <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="2">
-        <v>49</v>
-      </c>
+      <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
-      <c r="E49" s="32"/>
-      <c r="G49" s="2">
-        <v>49</v>
-      </c>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="2">
-        <v>50</v>
-      </c>
+      <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="G50" s="2">
-        <v>50</v>
-      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="2">
-        <v>51</v>
-      </c>
+      <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
-      <c r="G51" s="2">
-        <v>51</v>
-      </c>
+      <c r="E51" s="32"/>
+      <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="2">
-        <v>52</v>
-      </c>
+      <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
-      <c r="G52" s="2">
-        <v>52</v>
-      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="2">
-        <v>53</v>
-      </c>
+      <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
-      <c r="G53" s="2">
-        <v>53</v>
-      </c>
+      <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="2">
-        <v>54</v>
-      </c>
+      <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
-      <c r="G54" s="2">
-        <v>54</v>
-      </c>
+      <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="2">
-        <v>55</v>
-      </c>
+      <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
-      <c r="G55" s="2">
-        <v>55</v>
-      </c>
+      <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="2">
-        <v>56</v>
-      </c>
+      <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
-      <c r="G56" s="2">
-        <v>56</v>
-      </c>
+      <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="2">
-        <v>57</v>
-      </c>
+      <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
-      <c r="G57" s="2">
-        <v>57</v>
-      </c>
+      <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="2">
-        <v>58</v>
-      </c>
+      <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="4"/>
-      <c r="G58" s="2">
-        <v>58</v>
-      </c>
+      <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="2">
-        <v>59</v>
-      </c>
+      <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
-      <c r="G59" s="2">
-        <v>59</v>
-      </c>
+      <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="2">
-        <v>60</v>
-      </c>
+      <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
-      <c r="G60" s="2">
-        <v>60</v>
-      </c>
+      <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="2">
-        <v>61</v>
-      </c>
+      <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4"/>
-      <c r="G61" s="2">
-        <v>61</v>
-      </c>
+      <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="2">
-        <v>62</v>
-      </c>
+      <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
-      <c r="G62" s="2">
-        <v>62</v>
-      </c>
+      <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="2">
-        <v>63</v>
-      </c>
+      <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="4"/>
-      <c r="G63" s="2">
-        <v>63</v>
-      </c>
+      <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="2">
-        <v>64</v>
-      </c>
+      <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
-      <c r="G64" s="2">
-        <v>64</v>
-      </c>
+      <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="2">
-        <v>65</v>
-      </c>
+      <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
-      <c r="G65" s="2">
-        <v>65</v>
-      </c>
+      <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="2">
-        <v>66</v>
-      </c>
+      <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="4"/>
-      <c r="G66" s="2">
-        <v>66</v>
-      </c>
+      <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="2">
-        <v>67</v>
-      </c>
+      <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
-      <c r="G67" s="2">
-        <v>67</v>
-      </c>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="2">
-        <v>68</v>
-      </c>
+      <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="4"/>
-      <c r="G68" s="2">
-        <v>68</v>
-      </c>
+      <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="2">
-        <v>69</v>
-      </c>
+      <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="4"/>
-      <c r="G69" s="2">
-        <v>69</v>
-      </c>
+      <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="2">
-        <v>70</v>
-      </c>
+      <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="4"/>
-      <c r="G70" s="2">
-        <v>70</v>
-      </c>
+      <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="2">
-        <v>71</v>
-      </c>
+      <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="4"/>
-      <c r="G71" s="2">
-        <v>71</v>
-      </c>
+      <c r="G71" s="2"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="2">
-        <v>72</v>
-      </c>
+      <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
-      <c r="G72" s="2">
-        <v>72</v>
-      </c>
+      <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="2">
-        <v>73</v>
-      </c>
+      <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="4"/>
-      <c r="G73" s="2">
-        <v>73</v>
-      </c>
+      <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="2">
-        <v>74</v>
-      </c>
+      <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="4"/>
-      <c r="G74" s="2">
-        <v>74</v>
-      </c>
+      <c r="G74" s="2"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="2">
-        <v>75</v>
-      </c>
+      <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
-      <c r="G75" s="2">
-        <v>75</v>
-      </c>
+      <c r="G75" s="2"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="2">
-        <v>76</v>
-      </c>
+      <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
-      <c r="G76" s="2">
-        <v>76</v>
-      </c>
+      <c r="G76" s="2"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="2">
-        <v>77</v>
-      </c>
+      <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
-      <c r="G77" s="2">
-        <v>77</v>
-      </c>
+      <c r="G77" s="2"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="2">
-        <v>78</v>
-      </c>
+      <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
-      <c r="G78" s="2">
-        <v>78</v>
-      </c>
+      <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="2">
-        <v>79</v>
-      </c>
+      <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
-      <c r="G79" s="2">
-        <v>79</v>
-      </c>
+      <c r="G79" s="2"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="2">
-        <v>80</v>
-      </c>
+      <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
-      <c r="G80" s="2">
-        <v>80</v>
-      </c>
+      <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="2">
-        <v>81</v>
-      </c>
+      <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="4"/>
-      <c r="G81" s="2">
-        <v>81</v>
-      </c>
+      <c r="G81" s="2"/>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="2">
-        <v>82</v>
-      </c>
+      <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
-      <c r="G82" s="2">
-        <v>82</v>
-      </c>
+      <c r="G82" s="2"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="2">
-        <v>83</v>
-      </c>
+      <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="4"/>
-      <c r="G83" s="2">
-        <v>83</v>
-      </c>
+      <c r="G83" s="2"/>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="2">
-        <v>84</v>
-      </c>
+      <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="4"/>
-      <c r="G84" s="2">
-        <v>84</v>
-      </c>
+      <c r="G84" s="2"/>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="2">
-        <v>85</v>
-      </c>
+      <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
-      <c r="G85" s="2">
-        <v>85</v>
-      </c>
+      <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="2">
-        <v>86</v>
-      </c>
+      <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="4"/>
-      <c r="G86" s="2">
-        <v>86</v>
-      </c>
+      <c r="G86" s="2"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="2">
-        <v>87</v>
-      </c>
+      <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="4"/>
-      <c r="G87" s="2">
-        <v>87</v>
-      </c>
+      <c r="G87" s="2"/>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="2">
-        <v>88</v>
-      </c>
+      <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="4"/>
-      <c r="G88" s="2">
-        <v>88</v>
-      </c>
+      <c r="G88" s="2"/>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="2">
-        <v>89</v>
-      </c>
+      <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
-      <c r="G89" s="2">
-        <v>89</v>
-      </c>
+      <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="2">
-        <v>90</v>
-      </c>
+      <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="4"/>
-      <c r="G90" s="2">
-        <v>90</v>
-      </c>
+      <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="2">
-        <v>91</v>
-      </c>
+      <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="4"/>
-      <c r="G91" s="2">
-        <v>91</v>
-      </c>
+      <c r="G91" s="2"/>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="2">
-        <v>92</v>
-      </c>
+      <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="4"/>
-      <c r="G92" s="2">
-        <v>92</v>
-      </c>
+      <c r="G92" s="2"/>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="2">
-        <v>93</v>
-      </c>
+      <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="4"/>
-      <c r="G93" s="2">
-        <v>93</v>
-      </c>
+      <c r="G93" s="2"/>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="2">
-        <v>94</v>
-      </c>
+      <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="4"/>
-      <c r="G94" s="2">
-        <v>94</v>
-      </c>
+      <c r="G94" s="2"/>
     </row>
     <row r="95" spans="1:7">
-      <c r="A95" s="2">
-        <v>95</v>
-      </c>
+      <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="4"/>
-      <c r="G95" s="2">
-        <v>95</v>
-      </c>
+      <c r="G95" s="2"/>
     </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="2">
-        <v>96</v>
-      </c>
+      <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="4"/>
-      <c r="G96" s="2">
-        <v>96</v>
-      </c>
+      <c r="G96" s="2"/>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="2">
-        <v>97</v>
-      </c>
+      <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="4"/>
-      <c r="G97" s="2">
-        <v>97</v>
-      </c>
+      <c r="G97" s="2"/>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="2">
-        <v>98</v>
-      </c>
+      <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="4"/>
-      <c r="G98" s="2">
-        <v>98</v>
-      </c>
+      <c r="G98" s="2"/>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="2">
-        <v>99</v>
-      </c>
+      <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="4"/>
-      <c r="G99" s="2">
-        <v>99</v>
-      </c>
+      <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="2">
-        <v>100</v>
-      </c>
+      <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="4"/>
-      <c r="D100"/>
-      <c r="G100" s="2">
-        <v>100</v>
-      </c>
+      <c r="G100" s="2"/>
     </row>
     <row r="101" spans="1:7">
-      <c r="D101" s="24"/>
+      <c r="A101" s="2"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="4"/>
+      <c r="G101" s="2"/>
     </row>
     <row r="102" spans="1:7">
-      <c r="D102" s="24"/>
+      <c r="A102" s="2"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="4"/>
+      <c r="D102"/>
+      <c r="G102" s="2"/>
     </row>
     <row r="103" spans="1:7">
       <c r="D103" s="24"/>
     </row>
-    <row r="106" spans="1:7">
-      <c r="D106" s="24"/>
+    <row r="104" spans="1:7">
+      <c r="D104" s="24"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="D105" s="24"/>
     </row>
     <row r="108" spans="1:7">
-      <c r="E108" s="25"/>
+      <c r="D108" s="24"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="D110"/>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="D111" s="24"/>
+      <c r="E110" s="25"/>
     </row>
     <row r="112" spans="1:7">
-      <c r="D112" s="24"/>
+      <c r="D112"/>
     </row>
     <row r="113" spans="4:4">
       <c r="D113" s="24"/>
     </row>
     <row r="114" spans="4:4">
-      <c r="D114"/>
+      <c r="D114" s="24"/>
     </row>
     <row r="115" spans="4:4">
       <c r="D115" s="24"/>
     </row>
     <row r="116" spans="4:4">
-      <c r="D116" s="24"/>
+      <c r="D116"/>
     </row>
     <row r="117" spans="4:4">
       <c r="D117" s="24"/>
     </row>
     <row r="118" spans="4:4">
-      <c r="D118" s="9"/>
-    </row>
-    <row r="121" spans="4:4">
-      <c r="D121"/>
-    </row>
-    <row r="122" spans="4:4">
-      <c r="D122" s="24"/>
+      <c r="D118" s="24"/>
+    </row>
+    <row r="119" spans="4:4">
+      <c r="D119" s="24"/>
+    </row>
+    <row r="120" spans="4:4">
+      <c r="D120" s="9"/>
     </row>
     <row r="123" spans="4:4">
-      <c r="D123" s="24"/>
+      <c r="D123"/>
     </row>
     <row r="124" spans="4:4">
       <c r="D124" s="24"/>
     </row>
     <row r="125" spans="4:4">
-      <c r="D125"/>
+      <c r="D125" s="24"/>
     </row>
     <row r="126" spans="4:4">
       <c r="D126" s="24"/>
     </row>
     <row r="127" spans="4:4">
-      <c r="D127" s="24"/>
+      <c r="D127"/>
     </row>
     <row r="128" spans="4:4">
       <c r="D128" s="24"/>
     </row>
     <row r="129" spans="4:5">
-      <c r="D129" s="25"/>
-      <c r="E129" s="25"/>
-    </row>
-    <row r="132" spans="4:5">
-      <c r="E132" s="25"/>
+      <c r="D129" s="24"/>
+    </row>
+    <row r="130" spans="4:5">
+      <c r="D130" s="24"/>
+    </row>
+    <row r="131" spans="4:5">
+      <c r="D131" s="25"/>
+      <c r="E131" s="25"/>
     </row>
     <row r="134" spans="4:5">
       <c r="E134" s="25"/>
     </row>
-    <row r="137" spans="4:5">
-      <c r="D137"/>
-    </row>
-    <row r="138" spans="4:5">
-      <c r="D138" s="24"/>
+    <row r="136" spans="4:5">
+      <c r="E136" s="25"/>
     </row>
     <row r="139" spans="4:5">
-      <c r="D139" s="24"/>
+      <c r="D139"/>
     </row>
     <row r="140" spans="4:5">
       <c r="D140" s="24"/>
     </row>
     <row r="141" spans="4:5">
-      <c r="D141"/>
+      <c r="D141" s="24"/>
     </row>
     <row r="142" spans="4:5">
       <c r="D142" s="24"/>
     </row>
     <row r="143" spans="4:5">
-      <c r="D143" s="24"/>
+      <c r="D143"/>
     </row>
     <row r="144" spans="4:5">
       <c r="D144" s="24"/>
     </row>
     <row r="145" spans="4:5">
-      <c r="D145" s="25"/>
-      <c r="E145" s="25"/>
+      <c r="D145" s="24"/>
     </row>
     <row r="146" spans="4:5">
-      <c r="D146"/>
+      <c r="D146" s="24"/>
     </row>
     <row r="147" spans="4:5">
-      <c r="D147" s="24"/>
+      <c r="D147" s="25"/>
+      <c r="E147" s="25"/>
     </row>
     <row r="148" spans="4:5">
-      <c r="D148" s="24"/>
+      <c r="D148"/>
     </row>
     <row r="149" spans="4:5">
       <c r="D149" s="24"/>
     </row>
+    <row r="150" spans="4:5">
+      <c r="D150" s="24"/>
+    </row>
     <row r="151" spans="4:5">
-      <c r="E151" s="25"/>
-    </row>
-    <row r="152" spans="4:5">
-      <c r="D152" s="9"/>
-      <c r="E152" s="25"/>
+      <c r="D151" s="24"/>
     </row>
     <row r="153" spans="4:5">
       <c r="E153" s="25"/>
     </row>
     <row r="154" spans="4:5">
-      <c r="D154" s="25"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="25"/>
     </row>
     <row r="155" spans="4:5">
-      <c r="D155"/>
+      <c r="E155" s="25"/>
     </row>
     <row r="156" spans="4:5">
-      <c r="D156" s="24"/>
+      <c r="D156" s="25"/>
     </row>
     <row r="157" spans="4:5">
-      <c r="D157" s="24"/>
+      <c r="D157"/>
     </row>
     <row r="158" spans="4:5">
       <c r="D158" s="24"/>
     </row>
     <row r="159" spans="4:5">
-      <c r="D159"/>
+      <c r="D159" s="24"/>
     </row>
     <row r="160" spans="4:5">
       <c r="D160" s="24"/>
     </row>
     <row r="161" spans="4:5">
-      <c r="D161" s="24"/>
+      <c r="D161"/>
     </row>
     <row r="162" spans="4:5">
       <c r="D162" s="24"/>
     </row>
-    <row r="165" spans="4:5">
-      <c r="E165" s="25"/>
+    <row r="163" spans="4:5">
+      <c r="D163" s="24"/>
+    </row>
+    <row r="164" spans="4:5">
+      <c r="D164" s="24"/>
     </row>
     <row r="167" spans="4:5">
       <c r="E167" s="25"/>
     </row>
-    <row r="168" spans="4:5">
-      <c r="E168" s="25"/>
-    </row>
     <row r="169" spans="4:5">
       <c r="E169" s="25"/>
     </row>
-    <row r="175" spans="4:5">
-      <c r="E175" s="25"/>
+    <row r="170" spans="4:5">
+      <c r="E170" s="25"/>
+    </row>
+    <row r="171" spans="4:5">
+      <c r="E171" s="25"/>
     </row>
     <row r="177" spans="4:5">
       <c r="E177" s="25"/>
     </row>
-    <row r="178" spans="4:5">
-      <c r="E178" s="25"/>
-    </row>
     <row r="179" spans="4:5">
       <c r="E179" s="25"/>
     </row>
-    <row r="185" spans="4:5">
-      <c r="E185" s="25"/>
-    </row>
-    <row r="186" spans="4:5">
-      <c r="E186" s="25"/>
+    <row r="180" spans="4:5">
+      <c r="E180" s="25"/>
+    </row>
+    <row r="181" spans="4:5">
+      <c r="E181" s="25"/>
     </row>
     <row r="187" spans="4:5">
-      <c r="D187"/>
+      <c r="E187" s="25"/>
     </row>
     <row r="188" spans="4:5">
-      <c r="D188" s="24"/>
+      <c r="E188" s="25"/>
     </row>
     <row r="189" spans="4:5">
-      <c r="D189" s="24"/>
+      <c r="D189"/>
     </row>
     <row r="190" spans="4:5">
       <c r="D190" s="24"/>
     </row>
+    <row r="191" spans="4:5">
+      <c r="D191" s="24"/>
+    </row>
     <row r="192" spans="4:5">
-      <c r="D192" s="25"/>
-    </row>
-    <row r="193" spans="4:4">
-      <c r="D193" s="24"/>
-    </row>
-    <row r="197" spans="4:4">
-      <c r="D197"/>
+      <c r="D192" s="24"/>
+    </row>
+    <row r="194" spans="4:4">
+      <c r="D194" s="25"/>
+    </row>
+    <row r="195" spans="4:4">
+      <c r="D195" s="24"/>
+    </row>
+    <row r="199" spans="4:4">
+      <c r="D199"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D197" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <autoFilter ref="D1:D199" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -7765,13 +7605,13 @@
           <x14:formula1>
             <xm:f>Lookups!$U$3:$U$16</xm:f>
           </x14:formula1>
-          <xm:sqref>D154:D212 D51:D149 D23:D42 D46 D2:D15</xm:sqref>
+          <xm:sqref>D156:D214 D53:D151 D24:D44 D48 D2:D15 D20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Outcomes!$A$2:$A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B100</xm:sqref>
+          <xm:sqref>B2:B102</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>